<commit_message>
Abmeldung in Anmeldung heute Fenster; Null-Wert bei Abmeldung
</commit_message>
<xml_diff>
--- a/PythonCode/mysite/static/output.xlsx
+++ b/PythonCode/mysite/static/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="70">
   <si>
     <t>Vornamen</t>
   </si>
@@ -58,7 +58,7 @@
     <t>Soost</t>
   </si>
   <si>
-    <t>3C</t>
+    <t>3c</t>
   </si>
   <si>
     <t>4a</t>
@@ -175,6 +175,15 @@
     <t>18.12.2023 08:00</t>
   </si>
   <si>
+    <t>18.12.2023 09:53</t>
+  </si>
+  <si>
+    <t>20.12.2023 15:53</t>
+  </si>
+  <si>
+    <t>15.02.2024 13:43</t>
+  </si>
+  <si>
     <t>03.10.2023 20:01</t>
   </si>
   <si>
@@ -208,10 +217,13 @@
     <t>07.12.2023 20:41</t>
   </si>
   <si>
-    <t>18.12.2023 09:40</t>
-  </si>
-  <si>
-    <t>18.12.2023 08:01</t>
+    <t>18.12.2023 16:19</t>
+  </si>
+  <si>
+    <t>18.12.2023 16:20</t>
+  </si>
+  <si>
+    <t>15.02.2024 14:04</t>
   </si>
 </sst>
 </file>
@@ -569,7 +581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -609,7 +621,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F2">
         <v>49</v>
@@ -629,7 +641,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F3">
         <v>45</v>
@@ -649,7 +661,7 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F4">
         <v>44</v>
@@ -689,7 +701,7 @@
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F6">
         <v>93</v>
@@ -709,7 +721,7 @@
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F7">
         <v>93</v>
@@ -809,7 +821,7 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F12">
         <v>16</v>
@@ -829,7 +841,7 @@
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -909,7 +921,7 @@
         <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F17">
         <v>107</v>
@@ -929,7 +941,7 @@
         <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F18">
         <v>68</v>
@@ -949,7 +961,7 @@
         <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F19">
         <v>59</v>
@@ -969,7 +981,7 @@
         <v>32</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F20">
         <v>41</v>
@@ -1029,7 +1041,7 @@
         <v>35</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F23">
         <v>3</v>
@@ -1049,7 +1061,7 @@
         <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F24">
         <v>16</v>
@@ -1069,7 +1081,7 @@
         <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F25">
         <v>16</v>
@@ -1109,7 +1121,7 @@
         <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F27">
         <v>8</v>
@@ -1129,7 +1141,7 @@
         <v>39</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F28">
         <v>7</v>
@@ -1149,7 +1161,7 @@
         <v>40</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F29">
         <v>3</v>
@@ -1249,7 +1261,7 @@
         <v>45</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F34">
         <v>40</v>
@@ -1349,7 +1361,7 @@
         <v>50</v>
       </c>
       <c r="E39" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -1369,7 +1381,7 @@
         <v>50</v>
       </c>
       <c r="E40" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -1437,62 +1449,82 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D44" t="s">
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F44">
-        <v>100</v>
+        <v>499</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
         <v>15</v>
       </c>
       <c r="D45" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E46" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" t="s">
+        <v>69</v>
+      </c>
+      <c r="F47">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Schüler Anmeldehistorie; Haupseite ohne URL; ExportExcel auch Zeiten in DB auf 18 Uhr
</commit_message>
<xml_diff>
--- a/PythonCode/mysite/static/output.xlsx
+++ b/PythonCode/mysite/static/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="95">
   <si>
     <t>Vornamen</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Alex</t>
   </si>
   <si>
+    <t>Tim</t>
+  </si>
+  <si>
     <t>Fuchs</t>
   </si>
   <si>
@@ -79,6 +82,9 @@
     <t>Kross</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>3c</t>
   </si>
   <si>
@@ -97,6 +103,9 @@
     <t>10b</t>
   </si>
   <si>
+    <t>11c</t>
+  </si>
+  <si>
     <t>03.10.2023 19:12</t>
   </si>
   <si>
@@ -229,6 +238,9 @@
     <t>08.06.2024 21:31</t>
   </si>
   <si>
+    <t>15.06.2024 20:54</t>
+  </si>
+  <si>
     <t>03.10.2023 20:01</t>
   </si>
   <si>
@@ -277,13 +289,16 @@
     <t>08.06.2024 14:34</t>
   </si>
   <si>
-    <t>08.06.2024 18:00</t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t>08.06.2024 16:00</t>
+  </si>
+  <si>
+    <t>15.06.2024 18:00</t>
   </si>
   <si>
     <t>Automatisch</t>
+  </si>
+  <si>
+    <t>Abmeldung Automatisch</t>
   </si>
 </sst>
 </file>
@@ -641,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -675,22 +690,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F2">
         <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -698,22 +713,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F3">
         <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -721,22 +736,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F4">
         <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -744,22 +759,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -767,22 +782,22 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F6">
         <v>93</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -790,22 +805,22 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F7">
         <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -813,22 +828,22 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -836,22 +851,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F9">
         <v>44630</v>
       </c>
       <c r="G9" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -859,22 +874,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F10">
         <v>44630</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -882,22 +897,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F11">
         <v>44628</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -905,22 +920,22 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F12">
         <v>16</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -928,22 +943,22 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -951,22 +966,22 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -974,22 +989,22 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -997,22 +1012,22 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1020,22 +1035,22 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F17">
         <v>107</v>
       </c>
       <c r="G17" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1043,22 +1058,22 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F18">
         <v>68</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1066,22 +1081,22 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F19">
         <v>59</v>
       </c>
       <c r="G19" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1089,22 +1104,22 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F20">
         <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1112,22 +1127,22 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1135,22 +1150,22 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1158,22 +1173,22 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F23">
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1181,22 +1196,22 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F24">
         <v>16</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1204,22 +1219,22 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F25">
         <v>16</v>
       </c>
       <c r="G25" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1227,22 +1242,22 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1250,22 +1265,22 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F27">
         <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1273,22 +1288,22 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F28">
         <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1296,22 +1311,22 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F29">
         <v>3</v>
       </c>
       <c r="G29" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1319,22 +1334,22 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1342,22 +1357,22 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1365,22 +1380,22 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F32">
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1388,22 +1403,22 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F33">
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1411,22 +1426,22 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F34">
         <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1434,22 +1449,22 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F35">
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1457,22 +1472,22 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E36" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1480,22 +1495,22 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1503,22 +1518,22 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1526,22 +1541,22 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F39">
         <v>1</v>
       </c>
       <c r="G39" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1549,22 +1564,22 @@
         <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1572,22 +1587,22 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E41" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F41">
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1595,22 +1610,22 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E42" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1618,22 +1633,22 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E43" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1641,22 +1656,22 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E44" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F44">
         <v>499</v>
       </c>
       <c r="G44" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1664,22 +1679,22 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E45" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F45">
         <v>387</v>
       </c>
       <c r="G45" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1687,22 +1702,22 @@
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E46" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F46">
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1710,22 +1725,22 @@
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C47" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1733,22 +1748,22 @@
         <v>8</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1756,22 +1771,22 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E49" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1779,22 +1794,22 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E50" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F50">
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1802,22 +1817,22 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E51" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1825,22 +1840,22 @@
         <v>8</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D52" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E52" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F52">
         <v>4</v>
       </c>
       <c r="G52" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1848,22 +1863,22 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D53" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E53" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F53">
         <v>323</v>
       </c>
       <c r="G53" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1871,22 +1886,22 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D54" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E54" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F54">
         <v>740</v>
       </c>
       <c r="G54" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1894,22 +1909,22 @@
         <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D55" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E55" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F55">
         <v>418</v>
       </c>
       <c r="G55" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1917,22 +1932,22 @@
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C56" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D56" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E56" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F56">
-        <v>-209</v>
+        <v>-329</v>
       </c>
       <c r="G56" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1940,19 +1955,79 @@
         <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D57" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E57" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F57">
         <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" t="s">
+        <v>92</v>
+      </c>
+      <c r="F58">
+        <v>-174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" t="s">
+        <v>92</v>
+      </c>
+      <c r="F59">
+        <v>-174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" t="s">
+        <v>92</v>
+      </c>
+      <c r="F60">
+        <v>-174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixen, Farben Buttons vereinheitlicht, Buttons reduziert wie gewünscht
</commit_message>
<xml_diff>
--- a/PythonCode/mysite/static/output.xlsx
+++ b/PythonCode/mysite/static/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Vornamen</t>
+          <t>Vorname</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nachnamen</t>
+          <t>Nachname</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -473,17 +473,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Emmy</t>
+          <t>Stephan</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Watson</t>
+          <t>Fuchs</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2013a</t>
+          <t>2020B</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -493,64 +493,64 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>27.10.2024 19:52</t>
+          <t>27.10.2024 20:28</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Stephan</t>
+          <t>Steven</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Wolf</t>
+          <t>Mustermann</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2020b</t>
+          <t>2013A</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>27.10.2024 18:17</t>
+          <t>27.10.2024 18:18</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>27.10.2024 19:49</t>
+          <t>27.10.2024 18:24</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>Maike</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mustermann</t>
+          <t>perfect</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2013a</t>
+          <t>2010B</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>27.10.2024 18:18</t>
+          <t>27.10.2024 18:19</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -559,102 +559,133 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Maike</t>
+          <t>Max</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>perfect</t>
+          <t>Schmitz</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>2010b</t>
+          <t>2020A</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>27.10.2024 18:19</t>
+          <t>27.10.2024 18:20</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>27.10.2024 18:24</t>
+          <t>27.10.2024 18:20</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Otto</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Schmitz</t>
+          <t>Langnamenokidoki</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2020a</t>
+          <t>2015B</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>27.10.2024 18:20</t>
+          <t>27.10.2024 18:52</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>27.10.2024 18:20</t>
+          <t>27.10.2024 19:52</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Otto</t>
+          <t>Maike</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Langnamenokidoki</t>
+          <t>perfect</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2013b</t>
+          <t>2010B</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>27.10.2024 18:52</t>
+          <t>14.03.2025 18:35</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>27.10.2024 19:52</t>
+          <t>14.03.2025 21:36</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="G7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Testico</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2015A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>14.03.2025 19:05</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>14.03.2025 20:03</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>58</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>